<commit_message>
Update Excel templates and enhance data structure for school reports
- Updated existing Excel templates for 'Mầm Non', 'Tiểu Học', 'THCS', and 'THPT' to reflect new data fields and structure.
- Modified data definitions in JSON files to improve clarity and accuracy, including changes to field names and types.
- Adjusted column mappings in JSON files to align with updated Excel templates.
- Enhanced form validation logic to skip specific fields during data processing.
</commit_message>
<xml_diff>
--- a/public/templates/th.xlsx
+++ b/public/templates/th.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CBDE51-1504-421F-8BD6-3C71D3F82491}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241FA5F1-3282-4587-8640-991785446DD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17985" yWindow="1035" windowWidth="23280" windowHeight="25620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiểu học" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tiểu học'!$A$5:$S$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Tiểu học'!$5:$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tiểu học'!$A$3:$S$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Tiểu học'!$3:$5</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="37">
   <si>
     <t xml:space="preserve">Tổng </t>
   </si>
@@ -102,13 +102,7 @@
     <t>Hợp đồng hỗ trợ, phục vụ</t>
   </si>
   <si>
-    <t>Kế toán, văn thư, thủ quỹ, giáo vụ</t>
-  </si>
-  <si>
-    <t>Kế toán, văn thư,  thủ quỹ</t>
-  </si>
-  <si>
-    <t>Mức độ tự chủ chi thường xuyên (%)</t>
+    <t>Trường…...</t>
   </si>
   <si>
     <t>Nhu cầu năm 2026</t>
@@ -126,10 +120,6 @@
     <t>Hợp đồng chuyên môn nghiệp vụ</t>
   </si>
   <si>
-    <t>Dự toán thu năm 2026 
-(ĐVT: triệu đồng)</t>
-  </si>
-  <si>
     <t>Tổng số CB-GV-NV có mặt (tại thời điểm tháng 8/2025)</t>
   </si>
   <si>
@@ -140,9 +130,6 @@
   </si>
   <si>
     <t>PHỤ LỤC 2: SỐ LƯỢNG NGƯỜI LÀM VIỆC TRONG CÁC TRƯỜNG TIỂU HỌC CÔNG LẬP</t>
-  </si>
-  <si>
-    <t>(Kèm theo Văn bản số         /SNV-TCBC ngày      tháng 8 năm 2025 của Sở Nội vụ)</t>
   </si>
   <si>
     <t>Ghi chú</t>
@@ -181,10 +168,63 @@
     <t>Trong chỉ tiêu Hội đồng nhân dân giao theo hằng năm</t>
   </si>
   <si>
-    <t>PHƯỜNG XÃ ĐẶC KHU</t>
-  </si>
-  <si>
-    <t>NHÓM</t>
+    <r>
+      <t>Đơn vị nhóm 3 hoặc 4</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Đơn vị thuộc nhóm nào thì điền số 3 hoặc 4 vào ô tương ứng)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mức độ tự chủ chi thường xuyên (%) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(Đơn vị nhóm 3 thực hiện nội dung này, đơn vị nhóm 4 để trống ô này)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dự toán thu năm 2026 
+(ĐVT: triệu đồng)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(Đơn vị nhóm 3 thực hiện nội dung này, đơn vị nhóm 4 để trống ô này)</t>
+    </r>
+  </si>
+  <si>
+    <t>Kế toán, văn thư, thủ quỹ, giáo vụ, y tế</t>
+  </si>
+  <si>
+    <t>Xã, phường, đặc khu</t>
+  </si>
+  <si>
+    <t>Tổng số học sinh khuyết tật học hòa nhập</t>
+  </si>
+  <si>
+    <t>Kế toán, văn thư,  thủ quỹ, giáo vụ, y tế</t>
   </si>
 </sst>
 </file>
@@ -194,7 +234,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,12 +319,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="14"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -297,8 +331,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,8 +358,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -355,19 +408,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -458,15 +498,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -491,43 +522,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -536,43 +532,65 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -581,82 +599,52 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="8">
     <cellStyle name="Comma 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -665,7 +653,6 @@
     <cellStyle name="Normal 3 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal 5" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 5 2" xfId="8" xr:uid="{93A24B42-6BC3-6D41-8CBD-525C2EEBCD1B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1001,365 +988,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5:H7"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="40" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="40" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="40" customWidth="1"/>
-    <col min="5" max="7" width="8" style="40" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" style="40" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" style="40" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" style="40" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" style="40" customWidth="1"/>
-    <col min="12" max="14" width="6.140625" style="40" customWidth="1"/>
-    <col min="15" max="15" width="5.42578125" style="40" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="40" customWidth="1"/>
-    <col min="17" max="17" width="6.42578125" style="40" customWidth="1"/>
-    <col min="18" max="21" width="7.28515625" style="40" customWidth="1"/>
-    <col min="22" max="27" width="6.140625" style="40" customWidth="1"/>
-    <col min="28" max="29" width="7.85546875" style="40" customWidth="1"/>
-    <col min="30" max="30" width="6.140625" style="40" customWidth="1"/>
-    <col min="31" max="33" width="6.85546875" style="40" customWidth="1"/>
-    <col min="34" max="16384" width="8.85546875" style="40"/>
+    <col min="1" max="1" width="4.5703125" style="36" customWidth="1"/>
+    <col min="2" max="3" width="30.140625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="36" customWidth="1"/>
+    <col min="5" max="7" width="8" style="36" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" style="36" customWidth="1"/>
+    <col min="9" max="12" width="7.7109375" style="36" customWidth="1"/>
+    <col min="13" max="14" width="6.140625" style="36" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" style="36" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" style="36" customWidth="1"/>
+    <col min="17" max="17" width="6.5703125" style="36" customWidth="1"/>
+    <col min="18" max="21" width="7.28515625" style="36" customWidth="1"/>
+    <col min="22" max="26" width="6.140625" style="36" customWidth="1"/>
+    <col min="27" max="27" width="7.28515625" style="36" customWidth="1"/>
+    <col min="28" max="29" width="7.7109375" style="36" customWidth="1"/>
+    <col min="30" max="30" width="6.140625" style="36" customWidth="1"/>
+    <col min="31" max="33" width="6.85546875" style="36" customWidth="1"/>
+    <col min="34" max="34" width="11.7109375" style="36" customWidth="1"/>
+    <col min="35" max="35" width="16.5703125" style="36" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="41.25" hidden="1" customHeight="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:35" s="2" customFormat="1" ht="41.25" hidden="1" customHeight="1">
+      <c r="A1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
       <c r="S1" s="11"/>
       <c r="T1" s="11"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
       <c r="AB1" s="11"/>
       <c r="AC1" s="11"/>
       <c r="AD1" s="11"/>
     </row>
-    <row r="2" spans="1:34" s="3" customFormat="1" ht="15" customHeight="1"/>
-    <row r="3" spans="1:34" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A3" s="24" t="s">
+    <row r="2" spans="1:35" s="3" customFormat="1" ht="33.75" customHeight="1" thickBot="1">
+      <c r="A2" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="7"/>
+    </row>
+    <row r="3" spans="1:35" s="35" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A3" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="25"/>
+      <c r="M3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="32"/>
+      <c r="AH3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI3" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" s="35" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A4" s="24"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="33"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="20"/>
+    </row>
+    <row r="5" spans="1:35" s="35" customFormat="1" ht="167.45" customHeight="1">
+      <c r="A5" s="24"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="24"/>
-      <c r="AF3" s="24"/>
-      <c r="AG3" s="24"/>
+      <c r="AC5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH5" s="12"/>
+      <c r="AI5" s="20"/>
     </row>
-    <row r="4" spans="1:34" ht="19.5" thickBot="1">
-      <c r="A4" s="33" t="s">
+    <row r="6" spans="1:35" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="37">
+        <v>1</v>
+      </c>
+      <c r="B6" s="38">
+        <v>2</v>
+      </c>
+      <c r="C6" s="37">
+        <v>3</v>
+      </c>
+      <c r="D6" s="38">
+        <v>4</v>
+      </c>
+      <c r="E6" s="37">
+        <v>5</v>
+      </c>
+      <c r="F6" s="38">
+        <v>6</v>
+      </c>
+      <c r="G6" s="37">
+        <v>7</v>
+      </c>
+      <c r="H6" s="38">
+        <v>8</v>
+      </c>
+      <c r="I6" s="37">
+        <v>9</v>
+      </c>
+      <c r="J6" s="38">
+        <v>10</v>
+      </c>
+      <c r="K6" s="37">
+        <v>11</v>
+      </c>
+      <c r="L6" s="38">
+        <v>12</v>
+      </c>
+      <c r="M6" s="37">
+        <v>13</v>
+      </c>
+      <c r="N6" s="38">
+        <v>14</v>
+      </c>
+      <c r="O6" s="37">
+        <v>15</v>
+      </c>
+      <c r="P6" s="38">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="37">
+        <v>17</v>
+      </c>
+      <c r="R6" s="38">
+        <v>18</v>
+      </c>
+      <c r="S6" s="37">
+        <v>19</v>
+      </c>
+      <c r="T6" s="38">
+        <v>20</v>
+      </c>
+      <c r="U6" s="37">
+        <v>21</v>
+      </c>
+      <c r="V6" s="38">
+        <v>22</v>
+      </c>
+      <c r="W6" s="37">
+        <v>23</v>
+      </c>
+      <c r="X6" s="38">
+        <v>24</v>
+      </c>
+      <c r="Y6" s="37">
+        <v>25</v>
+      </c>
+      <c r="Z6" s="38">
+        <v>26</v>
+      </c>
+      <c r="AA6" s="37">
+        <v>27</v>
+      </c>
+      <c r="AB6" s="38">
+        <v>28</v>
+      </c>
+      <c r="AC6" s="37">
         <v>29</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="33"/>
-      <c r="AA4" s="33"/>
-      <c r="AB4" s="33"/>
-      <c r="AC4" s="33"/>
-      <c r="AD4" s="33"/>
-      <c r="AE4" s="33"/>
-      <c r="AF4" s="33"/>
-      <c r="AG4" s="33"/>
-    </row>
-    <row r="5" spans="1:34" s="41" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A5" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="28" t="s">
+      <c r="AD6" s="38">
+        <v>30</v>
+      </c>
+      <c r="AE6" s="37">
+        <v>31</v>
+      </c>
+      <c r="AF6" s="38">
+        <v>32</v>
+      </c>
+      <c r="AG6" s="37">
+        <v>33</v>
+      </c>
+      <c r="AH6" s="38">
         <v>34</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="AI6" s="37">
         <v>35</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="T5" s="36"/>
-      <c r="U5" s="36"/>
-      <c r="V5" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="16"/>
-      <c r="AD5" s="16"/>
-      <c r="AE5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF5" s="25"/>
-      <c r="AG5" s="30"/>
-      <c r="AH5" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" s="41" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="17"/>
-      <c r="AB6" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="26"/>
-      <c r="AG6" s="31"/>
-      <c r="AH6" s="13"/>
-    </row>
-    <row r="7" spans="1:34" s="41" customFormat="1" ht="138.6" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="U7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="W7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="X7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH7" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="V5:AD5"/>
-    <mergeCell ref="AD6:AD7"/>
-    <mergeCell ref="V6:AA6"/>
-    <mergeCell ref="S5:U6"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AH5:AH7"/>
+    <mergeCell ref="AI3:AI5"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="I5:J6"/>
-    <mergeCell ref="A3:AG3"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="AE5:AG6"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="I3:J4"/>
+    <mergeCell ref="A2:AG2"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="AE3:AG4"/>
     <mergeCell ref="V1:AA1"/>
     <mergeCell ref="M1:R1"/>
-    <mergeCell ref="K5:L6"/>
-    <mergeCell ref="A4:AG4"/>
-    <mergeCell ref="M5:R6"/>
+    <mergeCell ref="K3:L4"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="AH3:AH5"/>
+    <mergeCell ref="M3:R4"/>
+    <mergeCell ref="V3:AD3"/>
+    <mergeCell ref="AD4:AD5"/>
+    <mergeCell ref="V4:AA4"/>
+    <mergeCell ref="S3:U4"/>
+    <mergeCell ref="AB4:AC4"/>
   </mergeCells>
   <pageMargins left="7.874015748031496E-2" right="0" top="0.19685039370078741" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>